<commit_message>
Bump to Creek 2.1, keep parse speed optimization Merge remote-tracking branch 'upstream/master' into optimize-parse-speed Bring back hash for column names and indices mapping
</commit_message>
<xml_diff>
--- a/spec/fixtures/sample.xlsx
+++ b/spec/fixtures/sample.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maj/Development/TD/creek/spec/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="50600" windowHeight="16540" tabRatio="282"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="282"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -147,21 +155,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -487,15 +502,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ8"/>
+  <dimension ref="A1:AZ10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:52" ht="12" customHeight="1">
+    <row r="1" spans="1:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="12" customHeight="1">
+    <row r="2" spans="1:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -517,8 +532,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="12" customHeight="1"/>
-    <row r="4" spans="1:52" ht="12" customHeight="1">
+    <row r="3" spans="1:52" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="4" spans="1:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -538,7 +553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="12" customHeight="1">
+    <row r="5" spans="1:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z5" t="s">
         <v>19</v>
       </c>
@@ -546,7 +561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="12" customHeight="1">
+    <row r="6" spans="1:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -558,28 +573,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="12" customHeight="1">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="12" customHeight="1">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
       <c r="F8" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.15">
+      <c r="A10" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>
@@ -592,10 +615,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>